<commit_message>
update fix mot so loi
</commit_message>
<xml_diff>
--- a/Files/student_in_class.xlsx
+++ b/Files/student_in_class.xlsx
@@ -37,7 +37,7 @@
     <t xml:space="preserve">Phan Nguyễn Đăng Trường</t>
   </si>
   <si>
-    <t xml:space="preserve">truongpnd@fe.fpt.vn</t>
+    <t xml:space="preserve">truongpndps16501@fpt.edu.vn</t>
   </si>
   <si>
     <t xml:space="preserve">PS5555</t>
@@ -242,7 +242,7 @@
   <dimension ref="A1:C1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K8" activeCellId="0" sqref="K8"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -298,7 +298,7 @@
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="truongpnd@fe.fpt.vn"/>
+    <hyperlink ref="C2" r:id="rId1" display="truongpndps16501@fpt.edu.vn"/>
     <hyperlink ref="C3" r:id="rId2" display="duydh@fe.fpt.vn"/>
     <hyperlink ref="C4" r:id="rId3" display="thangnnc@fe.fpt.vn"/>
   </hyperlinks>

</xml_diff>